<commit_message>
A little bit of clean up.
Signed-off-by: Connor Graydon <connorj@bully4u.com>
</commit_message>
<xml_diff>
--- a/chinuk_vocab_gold.xlsx
+++ b/chinuk_vocab_gold.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Desktop/chinuk_vocab_repo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Desktop/chinuk_repos/chinuk_vocab_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEA7DD8B-43E7-634F-9317-845412E54C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A052436A-C879-5C4E-84EA-0DE116BD14FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45220" yWindow="2160" windowWidth="42140" windowHeight="26680" activeTab="17" xr2:uid="{7DFB5DAA-41FE-8F4C-ADA0-7B74441B15D5}"/>
+    <workbookView minimized="1" xWindow="-45220" yWindow="2160" windowWidth="42140" windowHeight="26680" activeTab="20" xr2:uid="{7DFB5DAA-41FE-8F4C-ADA0-7B74441B15D5}"/>
   </bookViews>
   <sheets>
     <sheet name="question_words" sheetId="8" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="1454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="1455">
   <si>
     <t>tʼsiqʰwaʔ</t>
   </si>
@@ -4421,6 +4421,9 @@
   </si>
   <si>
     <t>iqʰix</t>
+  </si>
+  <si>
+    <t>These came from plant presentations in cw103 in spring 2023 (I think).</t>
   </si>
 </sst>
 </file>
@@ -4710,7 +4713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4794,16 +4797,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5121,7 +5120,7 @@
   <dimension ref="A2:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -5340,60 +5339,60 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="26">
-      <c r="F20" s="45" t="s">
+      <c r="F20" s="44" t="s">
         <v>1181</v>
       </c>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="44" t="s">
         <v>1182</v>
       </c>
-      <c r="H20" s="45"/>
+      <c r="H20" s="44"/>
     </row>
     <row r="21" spans="1:8" ht="26">
-      <c r="F21" s="45" t="s">
+      <c r="F21" s="44" t="s">
         <v>1183</v>
       </c>
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="44" t="s">
         <v>1184</v>
       </c>
-      <c r="H21" s="45"/>
+      <c r="H21" s="44"/>
     </row>
     <row r="22" spans="1:8" ht="26">
-      <c r="F22" s="45" t="s">
+      <c r="F22" s="44" t="s">
         <v>1185</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="44" t="s">
         <v>1186</v>
       </c>
-      <c r="H22" s="45"/>
+      <c r="H22" s="44"/>
     </row>
     <row r="23" spans="1:8" ht="26">
-      <c r="F23" s="45" t="s">
+      <c r="F23" s="44" t="s">
         <v>1189</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="44" t="s">
         <v>1190</v>
       </c>
-      <c r="H23" s="45"/>
+      <c r="H23" s="44"/>
     </row>
     <row r="24" spans="1:8" ht="26">
-      <c r="F24" s="45" t="s">
+      <c r="F24" s="44" t="s">
         <v>1179</v>
       </c>
-      <c r="G24" s="45" t="s">
+      <c r="G24" s="44" t="s">
         <v>1180</v>
       </c>
-      <c r="H24" s="45" t="s">
+      <c r="H24" s="44" t="s">
         <v>1191</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="26">
-      <c r="F25" s="45" t="s">
+      <c r="F25" s="44" t="s">
         <v>1192</v>
       </c>
-      <c r="G25" s="45" t="s">
+      <c r="G25" s="44" t="s">
         <v>1193</v>
       </c>
-      <c r="H25" s="45"/>
+      <c r="H25" s="44"/>
     </row>
     <row r="26" spans="1:8" ht="24">
       <c r="F26" s="23"/>
@@ -6161,10 +6160,10 @@
         <v>81</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="48" t="s">
+      <c r="G22" s="45" t="s">
         <v>524</v>
       </c>
-      <c r="H22" s="48" t="s">
+      <c r="H22" s="45" t="s">
         <v>525</v>
       </c>
       <c r="I22" s="4"/>
@@ -6583,8 +6582,8 @@
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -8705,7 +8704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8189FA-8DE2-CE4D-844B-A846D91C12A6}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -9137,7 +9136,7 @@
         <v>1350</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="46" t="s">
         <v>1351</v>
       </c>
     </row>
@@ -9445,10 +9444,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1446148E-86CD-C745-8E28-605EED3FB402}">
-  <dimension ref="A2:B64"/>
+  <dimension ref="A2:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -9457,23 +9456,25 @@
     <col min="2" max="2" width="64.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="24">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:4" ht="24">
+      <c r="A2" s="43" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="24">
-      <c r="A3" s="43"/>
-    </row>
-    <row r="4" spans="1:2" ht="24">
-      <c r="A4" s="24" t="s">
+    <row r="3" spans="1:4">
+      <c r="D3" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="24">
+      <c r="A4" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="24">
+    <row r="5" spans="1:4" ht="24">
       <c r="A5" s="21" t="s">
         <v>605</v>
       </c>
@@ -9481,7 +9482,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="24">
+    <row r="6" spans="1:4" ht="24">
       <c r="A6" s="21" t="s">
         <v>606</v>
       </c>
@@ -9489,7 +9490,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="24">
+    <row r="7" spans="1:4" ht="24">
       <c r="A7" s="21" t="s">
         <v>607</v>
       </c>
@@ -9497,7 +9498,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="24">
+    <row r="8" spans="1:4" ht="24">
       <c r="A8" s="21" t="s">
         <v>608</v>
       </c>
@@ -9505,7 +9506,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="24">
+    <row r="9" spans="1:4" ht="24">
       <c r="A9" s="21" t="s">
         <v>609</v>
       </c>
@@ -9513,7 +9514,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="24">
+    <row r="10" spans="1:4" ht="24">
       <c r="A10" s="21" t="s">
         <v>610</v>
       </c>
@@ -9521,7 +9522,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="24">
+    <row r="11" spans="1:4" ht="24">
       <c r="A11" s="21" t="s">
         <v>662</v>
       </c>
@@ -9529,7 +9530,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="24">
+    <row r="12" spans="1:4" ht="24">
       <c r="A12" s="21" t="s">
         <v>611</v>
       </c>
@@ -9537,7 +9538,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="24">
+    <row r="13" spans="1:4" ht="24">
       <c r="A13" s="21" t="s">
         <v>612</v>
       </c>
@@ -9545,7 +9546,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="24">
+    <row r="14" spans="1:4" ht="24">
       <c r="A14" s="21" t="s">
         <v>613</v>
       </c>
@@ -9553,7 +9554,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="24">
+    <row r="15" spans="1:4" ht="24">
       <c r="A15" s="21" t="s">
         <v>614</v>
       </c>
@@ -9561,7 +9562,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="24">
+    <row r="16" spans="1:4" ht="24">
       <c r="A16" s="21" t="s">
         <v>615</v>
       </c>

</xml_diff>